<commit_message>
inclui arquivos estimativas e consolidado UST
</commit_message>
<xml_diff>
--- a/usts-consolidados.xlsx
+++ b/usts-consolidados.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11730"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11730" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="43">
   <si>
     <t>grador de site estático</t>
   </si>
@@ -87,6 +88,72 @@
   </si>
   <si>
     <t>equipe</t>
+  </si>
+  <si>
+    <t>sprints</t>
+  </si>
+  <si>
+    <t>equipe_num</t>
+  </si>
+  <si>
+    <t>semanas</t>
+  </si>
+  <si>
+    <t>usts_equipe</t>
+  </si>
+  <si>
+    <t>usts_individuais</t>
+  </si>
+  <si>
+    <t>usts_totais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentação e apresentação (80), </t>
+  </si>
+  <si>
+    <t xml:space="preserve">identidade visual (30), </t>
+  </si>
+  <si>
+    <t xml:space="preserve">acompanhamento do scrum master (28), </t>
+  </si>
+  <si>
+    <t xml:space="preserve">arquitetura/definições(20), </t>
+  </si>
+  <si>
+    <t xml:space="preserve">implementação front-end (19), </t>
+  </si>
+  <si>
+    <t xml:space="preserve">entendimento, refinamento, escrita e validação (14), </t>
+  </si>
+  <si>
+    <t>guia usabilidade (10),</t>
+  </si>
+  <si>
+    <t>prototipação (9),</t>
+  </si>
+  <si>
+    <t>preparação e implementação (8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentação e apresentação (48), </t>
+  </si>
+  <si>
+    <t xml:space="preserve">implementação front-end ou back end (19), </t>
+  </si>
+  <si>
+    <t xml:space="preserve">identidade visual (15), </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prototipação (9), </t>
+  </si>
+  <si>
+    <t xml:space="preserve">preparação e implementação (8), </t>
+  </si>
+  <si>
+    <t>guia usabilidade (5)</t>
+  </si>
+  <si>
+    <t>historias</t>
   </si>
 </sst>
 </file>
@@ -415,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1082,4 +1149,177 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="49.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>640</v>
+      </c>
+      <c r="G2">
+        <v>2260</v>
+      </c>
+      <c r="H2">
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>12</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>162</v>
+      </c>
+      <c r="G3">
+        <f>H3-F3</f>
+        <v>688</v>
+      </c>
+      <c r="H3">
+        <v>850</v>
+      </c>
+      <c r="J3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="J4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>31</v>
+      </c>
+      <c r="K8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>32</v>
+      </c>
+      <c r="K9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>